<commit_message>
Css changed in properties file
Css changed in properties file due to change in code.
</commit_message>
<xml_diff>
--- a/test-output/SuiteReport.xlsx
+++ b/test-output/SuiteReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Category</t>
   </si>
@@ -42,19 +42,19 @@
     <t>Start Time</t>
   </si>
   <si>
-    <t>2018-07-15T16:15:39Z</t>
+    <t>2018-07-16T06:31:26Z</t>
   </si>
   <si>
     <t>End Time</t>
   </si>
   <si>
-    <t>2018-07-15T16:16:00Z</t>
+    <t>2018-07-16T06:31:56Z</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>20438 ms</t>
+    <t>30607 ms</t>
   </si>
   <si>
     <t>TestCase Name</t>
@@ -72,16 +72,23 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>expected [true] but found [false]</t>
-  </si>
-  <si>
-    <t>2018-07-15T16:15:53Z</t>
-  </si>
-  <si>
-    <t>2018-07-15T16:15:59Z</t>
-  </si>
-  <si>
-    <t>5871 ms</t>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":".menu.clearfix &gt; li:nth-child(3) &gt; ul &gt; li:nth-child(2) &gt; ul &gt; li:nth-child(5) &gt; a"}
+  (Session info: chrome=67.0.3396.99)
+  (Driver info: chromedriver=2.40.565498 (ea082db3280dd6843ebfb08a625e3eb905c4f5ab),platform=Windows NT 10.0.15063 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.11.0', revision: 'e59cfb3', time: '2018-03-11T20:33:08.638Z'
+System info: host: 'LIPL-HO-L-088', ip: '192.168.18.116', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_171'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.40.565498 (ea082db3280dd6..., userDataDir: C:\Users\LOKESH~1.SHA\AppDa...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 67.0.3396.99, webStorageEnabled: true}
+Session ID: d7f08faf953b50c54e2ffda55781eaf5
+*** Element info: {Using=css selector, value=.menu.clearfix &gt; li:nth-child(3) &gt; ul &gt; li:nth-child(2) &gt; ul &gt; li:nth-child(5) &gt; a}</t>
+  </si>
+  <si>
+    <t>2018-07-16T06:31:46Z</t>
+  </si>
+  <si>
+    <t>9337 ms</t>
   </si>
 </sst>
 </file>
@@ -291,7 +298,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="13.88671875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="27.078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="27.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -375,9 +382,9 @@
   <cols>
     <col min="1" max="1" width="62.3984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.6171875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.9140625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="27.078125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="27.078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="27.46484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="27.46484375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.08203125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -415,10 +422,10 @@
         <v>20</v>
       </c>
       <c r="E2" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="30" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>